<commit_message>
Simplify and clarify scenario names
Former-commit-id: f215409fb525dffd4937e1e76170dfe23371f536
</commit_message>
<xml_diff>
--- a/images/linktable.xlsx
+++ b/images/linktable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxbarnes/Documents/GitHub/resiliency_paper/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregmacfarlane/projects/resiliency_paper/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9D749F5-0EAF-044F-A288-FE56F7C04E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5580813-73B4-9445-B00E-203281217717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="3000" windowWidth="26840" windowHeight="15940" xr2:uid="{6F16606E-365F-B244-8227-3D442C4BD5A3}"/>
+    <workbookView xWindow="39680" yWindow="3040" windowWidth="33460" windowHeight="28520" xr2:uid="{6F16606E-365F-B244-8227-3D442C4BD5A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,87 +51,54 @@
     <t>SR-95</t>
   </si>
   <si>
-    <t>near Hite</t>
-  </si>
-  <si>
     <t>road11</t>
   </si>
   <si>
     <t>US-6</t>
   </si>
   <si>
-    <t>near King Top</t>
-  </si>
-  <si>
     <t>road12</t>
   </si>
   <si>
     <t>I-15</t>
   </si>
   <si>
-    <t>in Bountiful</t>
-  </si>
-  <si>
     <t>road13</t>
   </si>
   <si>
     <t>I-70</t>
   </si>
   <si>
-    <t>at Dragon Point (W of Green River)</t>
-  </si>
-  <si>
     <t>road14</t>
   </si>
   <si>
-    <t>in Orem between Univ. Ave &amp; Center St</t>
-  </si>
-  <si>
     <t>road15</t>
   </si>
   <si>
     <t>SR-199</t>
   </si>
   <si>
-    <t>near Rush Valley</t>
-  </si>
-  <si>
     <t>road16</t>
   </si>
   <si>
     <t>SR-153</t>
   </si>
   <si>
-    <t>between Beaver &amp; Junction</t>
-  </si>
-  <si>
     <t>road17</t>
   </si>
   <si>
     <t>SR-18</t>
   </si>
   <si>
-    <t>just North of St. George</t>
-  </si>
-  <si>
     <t>road18</t>
   </si>
   <si>
-    <t>near Rocky Ridge (between Payson &amp; Nephi)</t>
-  </si>
-  <si>
     <t>road19</t>
   </si>
   <si>
-    <t>near I-70 &amp; Filmore</t>
-  </si>
-  <si>
     <t>road20</t>
   </si>
   <si>
-    <t xml:space="preserve">near New Harmony </t>
-  </si>
-  <si>
     <t>road21</t>
   </si>
   <si>
@@ -144,99 +111,66 @@
     <t>road22</t>
   </si>
   <si>
-    <t>in Carbon County North of Helper</t>
-  </si>
-  <si>
     <t>road23</t>
   </si>
   <si>
     <t>Legacy Parkway</t>
   </si>
   <si>
-    <t>near West Bountiful</t>
-  </si>
-  <si>
     <t>road24</t>
   </si>
   <si>
     <t>UT-35</t>
   </si>
   <si>
-    <t>outside of Francis</t>
-  </si>
-  <si>
     <t>road25</t>
   </si>
   <si>
     <t>Timp Highway</t>
   </si>
   <si>
-    <t>at the base of AF Canyon</t>
-  </si>
-  <si>
     <t>road26</t>
   </si>
   <si>
     <t>SR-14</t>
   </si>
   <si>
-    <t>in Cedar Canyon</t>
-  </si>
-  <si>
     <t>road27</t>
   </si>
   <si>
     <t>I-84</t>
   </si>
   <si>
-    <t>between Ogden and Morgan</t>
-  </si>
-  <si>
     <t>road28</t>
   </si>
   <si>
     <t>SR-65</t>
   </si>
   <si>
-    <t>on the border of Salt Lake County &amp; Morgan County</t>
-  </si>
-  <si>
     <t>road29</t>
   </si>
   <si>
     <t>SR-101</t>
   </si>
   <si>
-    <t>East of Hyrum</t>
-  </si>
-  <si>
     <t>road30</t>
   </si>
   <si>
     <t>US-91</t>
   </si>
   <si>
-    <t>between Brigham City &amp; Mantua</t>
-  </si>
-  <si>
     <t>road31</t>
   </si>
   <si>
     <t>SR-62</t>
   </si>
   <si>
-    <t>East of Kingston</t>
-  </si>
-  <si>
     <t>road32</t>
   </si>
   <si>
     <t>US-89</t>
   </si>
   <si>
-    <t>between Logan and Bear Lake</t>
-  </si>
-  <si>
     <t>road33</t>
   </si>
   <si>
@@ -267,103 +201,169 @@
     <t>road36</t>
   </si>
   <si>
-    <t>near Steamboat Point</t>
-  </si>
-  <si>
     <t>road37</t>
   </si>
   <si>
     <t>I-80</t>
   </si>
   <si>
-    <t>in Parley's Canyon</t>
-  </si>
-  <si>
     <t>road38</t>
   </si>
   <si>
-    <t>at the Point of the Mountain</t>
-  </si>
-  <si>
     <t>road39</t>
   </si>
   <si>
-    <t>in SLC near Sugar House and 1300 E</t>
-  </si>
-  <si>
     <t>road40</t>
   </si>
   <si>
-    <t>in SLC between 2100 S &amp; 1300 S</t>
-  </si>
-  <si>
     <t>road41</t>
   </si>
   <si>
     <t>I-215</t>
   </si>
   <si>
-    <t>near Taylorsville</t>
-  </si>
-  <si>
     <t>road42</t>
   </si>
   <si>
-    <t>near West Valley City</t>
-  </si>
-  <si>
     <t>road43</t>
   </si>
   <si>
-    <t>near Cottonwood Heights</t>
-  </si>
-  <si>
     <t>road44</t>
   </si>
   <si>
     <t>MVC (UT-85)</t>
   </si>
   <si>
-    <t>West of West Jordan</t>
-  </si>
-  <si>
     <t>road45</t>
   </si>
   <si>
-    <t>near the Border of Arizona by Lake Powell</t>
-  </si>
-  <si>
     <t>road46</t>
   </si>
   <si>
     <t>SR-189</t>
   </si>
   <si>
-    <t>up Provo Canyon near Vivian Park</t>
-  </si>
-  <si>
     <t>road47</t>
   </si>
   <si>
-    <t>up Spanish Fork Canyon near Diamond Fork Rd</t>
-  </si>
-  <si>
     <t>road48</t>
   </si>
   <si>
-    <t>near Green River (NW of Moab)</t>
-  </si>
-  <si>
     <t>road49</t>
   </si>
   <si>
-    <t>near Richfield &amp; Filmore</t>
-  </si>
-  <si>
     <t>road50</t>
   </si>
   <si>
-    <t>between SLC and Tooele</t>
+    <t>Hite</t>
+  </si>
+  <si>
+    <t>King Top</t>
+  </si>
+  <si>
+    <t>Bountiful</t>
+  </si>
+  <si>
+    <t>West of Green River</t>
+  </si>
+  <si>
+    <t>Orem</t>
+  </si>
+  <si>
+    <t>Rush Valley</t>
+  </si>
+  <si>
+    <t>Beaver Canyon</t>
+  </si>
+  <si>
+    <t>Snow Canyon</t>
+  </si>
+  <si>
+    <t>North of Cove Fort</t>
+  </si>
+  <si>
+    <t>North of Zion</t>
+  </si>
+  <si>
+    <t>Price Canyon</t>
+  </si>
+  <si>
+    <t>West Bountiful</t>
+  </si>
+  <si>
+    <t>Francis</t>
+  </si>
+  <si>
+    <t>American Fork Canyon</t>
+  </si>
+  <si>
+    <t>Cedar Canyon</t>
+  </si>
+  <si>
+    <t>Weber Canyon</t>
+  </si>
+  <si>
+    <t>Emigration Canyon</t>
+  </si>
+  <si>
+    <t>Hyrum</t>
+  </si>
+  <si>
+    <t>Logan Canyon</t>
+  </si>
+  <si>
+    <t>Kingston</t>
+  </si>
+  <si>
+    <t>Box Elder Canyon</t>
+  </si>
+  <si>
+    <t>West of Hanksville</t>
+  </si>
+  <si>
+    <t>Parley's Canyon</t>
+  </si>
+  <si>
+    <t>SLC 1300 E</t>
+  </si>
+  <si>
+    <t>Taylorsville</t>
+  </si>
+  <si>
+    <t>West Valley City</t>
+  </si>
+  <si>
+    <t>Cottonwood Heights</t>
+  </si>
+  <si>
+    <t>West Jordan</t>
+  </si>
+  <si>
+    <t>Arizona state line</t>
+  </si>
+  <si>
+    <t>Provo Canyon</t>
+  </si>
+  <si>
+    <t>Spanish Fork Canyon</t>
+  </si>
+  <si>
+    <t>Colorado state line</t>
+  </si>
+  <si>
+    <t>Utah / Juab county line</t>
+  </si>
+  <si>
+    <t>Utah / Salt Lake county line</t>
+  </si>
+  <si>
+    <t>SLC  2100 S</t>
+  </si>
+  <si>
+    <t>East of Cove Fort</t>
+  </si>
+  <si>
+    <t>Salt Lake / Tooele county line</t>
   </si>
 </sst>
 </file>
@@ -730,10 +730,13 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C42"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="43.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -754,411 +757,411 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>103</v>
@@ -1166,32 +1169,32 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>109</v>

</xml_diff>